<commit_message>
Completada parte 3 de la práctica 2
</commit_message>
<xml_diff>
--- a/practicas/practica2/resultados.xlsx
+++ b/practicas/practica2/resultados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51440" yWindow="2040" windowWidth="23160" windowHeight="16960" tabRatio="500"/>
+    <workbookView xWindow="8280" yWindow="2040" windowWidth="17320" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i5-4570 (lab102-205)" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>Versión</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ICC</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>cond_esc</t>
+  </si>
+  <si>
+    <t>cond_vec</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,8 +657,8 @@
         <v>211865.765625</v>
       </c>
       <c r="J2" s="9">
-        <f t="shared" ref="J2:J17" si="0">$F$4/F2</f>
-        <v>0.22763010108573567</v>
+        <f>$F$5/F2</f>
+        <v>3.4444028453762633E-2</v>
       </c>
       <c r="K2" s="7">
         <f>D2/100/F2</f>
@@ -682,8 +694,8 @@
         <v>209818.6875</v>
       </c>
       <c r="J3" s="9">
-        <f t="shared" si="0"/>
-        <v>0.99346405228758172</v>
+        <f t="shared" ref="J3:J11" si="0">$F$5/F3</f>
+        <v>0.15032679738562091</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" ref="K3:K17" si="1">D3/100/F3</f>
@@ -720,7 +732,7 @@
       </c>
       <c r="J4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.15131578947368421</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="1"/>
@@ -757,7 +769,7 @@
       </c>
       <c r="J5" s="9">
         <f t="shared" si="0"/>
-        <v>6.6086956521739131</v>
+        <v>1</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="1"/>
@@ -794,7 +806,7 @@
       </c>
       <c r="J6" s="9">
         <f t="shared" si="0"/>
-        <v>6.5376344086021501</v>
+        <v>0.989247311827957</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="1"/>
@@ -831,7 +843,7 @@
       </c>
       <c r="J7" s="9">
         <f t="shared" si="0"/>
-        <v>6.6086956521739131</v>
+        <v>1</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
@@ -868,7 +880,7 @@
       </c>
       <c r="J8" s="9">
         <f t="shared" si="0"/>
-        <v>5.4285714285714279</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="1"/>
@@ -905,7 +917,7 @@
       </c>
       <c r="J9" s="9">
         <f t="shared" si="0"/>
-        <v>5.4774774774774775</v>
+        <v>0.8288288288288288</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
@@ -942,7 +954,7 @@
       </c>
       <c r="J10" s="9">
         <f t="shared" si="0"/>
-        <v>7.4146341463414638</v>
+        <v>1.1219512195121952</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="1"/>
@@ -979,7 +991,7 @@
       </c>
       <c r="J11" s="9">
         <f t="shared" si="0"/>
-        <v>6.6086956521739131</v>
+        <v>1</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="1"/>
@@ -1015,8 +1027,8 @@
         <v>956991104</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2771535580524347</v>
+        <f>$F$12/F12</f>
+        <v>1</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="1"/>
@@ -1052,8 +1064,8 @@
         <v>956523840</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2771535580524347</v>
+        <f t="shared" ref="J13:J15" si="2">$F$12/F13</f>
+        <v>1</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="1"/>
@@ -1089,8 +1101,8 @@
         <v>956991104</v>
       </c>
       <c r="J14" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2857142857142856</v>
+        <f t="shared" si="2"/>
+        <v>1.0037593984962405</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="1"/>
@@ -1126,8 +1138,8 @@
         <v>956523840</v>
       </c>
       <c r="J15" s="9">
-        <f t="shared" si="0"/>
-        <v>1.8881987577639752</v>
+        <f t="shared" si="2"/>
+        <v>0.82919254658385089</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="1"/>
@@ -1163,8 +1175,8 @@
         <v>478508800</v>
       </c>
       <c r="J16" s="9">
-        <f t="shared" si="0"/>
-        <v>1.6084656084656086</v>
+        <f>$F$16/F16</f>
+        <v>1</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="1"/>
@@ -1200,12 +1212,160 @@
         <v>478508800</v>
       </c>
       <c r="J17" s="9">
-        <f t="shared" si="0"/>
-        <v>1.6170212765957448</v>
+        <f>$F$16/F17</f>
+        <v>1.0053191489361701</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="1"/>
         <v>5.3191489361702127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3.54</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I18" s="2">
+        <v>478502976</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" ref="J18:J21" si="3">$F$16/F18</f>
+        <v>1.0677966101694916</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" ref="K18:K21" si="4">D18/100/F18</f>
+        <v>5.6497175141242941</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3.54</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I19" s="2">
+        <v>478502976</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="3"/>
+        <v>1.0677966101694916</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="4"/>
+        <v>5.6497175141242941</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I20" s="2">
+        <v>102.3685</v>
+      </c>
+      <c r="J20" s="9">
+        <f>$F$20/F20</f>
+        <v>1</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="4"/>
+        <v>3.6363636363636362</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1023.693359</v>
+      </c>
+      <c r="J21" s="9">
+        <f>$F$20/F21</f>
+        <v>3.4375</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>